<commit_message>
feat: Add Telegram field to employee contact section and import template
</commit_message>
<xml_diff>
--- a/public/templates/employeeImportTemplate.xlsx
+++ b/public/templates/employeeImportTemplate.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,39 +416,42 @@
         <v>Số điện thoại</v>
       </c>
       <c r="E1" t="str">
+        <v>Telegram</v>
+      </c>
+      <c r="F1" t="str">
         <v>Mã đơn vị *</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>Chức vụ</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>Role *</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>Ngày sinh</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>Giới tính</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" t="str">
         <v>Số CCCD</v>
       </c>
-      <c r="K1" t="str">
+      <c r="L1" t="str">
         <v>Địa chỉ</v>
       </c>
-      <c r="L1" t="str">
+      <c r="M1" t="str">
         <v>Trình độ học vấn</v>
       </c>
-      <c r="M1" t="str">
+      <c r="N1" t="str">
         <v>Ngày vào làm</v>
       </c>
-      <c r="N1" t="str">
+      <c r="O1" t="str">
         <v>Loại hợp đồng</v>
       </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
         <v>Số tài khoản NH</v>
       </c>
-      <c r="P1" t="str">
+      <c r="Q1" t="str">
         <v>Tên ngân hàng</v>
       </c>
     </row>
@@ -466,45 +469,48 @@
         <v>0901234567</v>
       </c>
       <c r="E2" t="str">
+        <v>@nguyen_a</v>
+      </c>
+      <c r="F2" t="str">
         <v>bim</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" t="str">
         <v>Chuyên viên</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
         <v>NVKD</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <v>15/03/1990</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" t="str">
         <v>Nam</v>
       </c>
-      <c r="J2" t="str">
+      <c r="K2" t="str">
         <v>001234567890</v>
       </c>
-      <c r="K2" t="str">
+      <c r="L2" t="str">
         <v>Hà Nội</v>
       </c>
-      <c r="L2" t="str">
+      <c r="M2" t="str">
         <v>Đại học</v>
       </c>
-      <c r="M2" t="str">
+      <c r="N2" t="str">
         <v>01/01/2024</v>
       </c>
-      <c r="N2" t="str">
+      <c r="O2" t="str">
         <v>Chính thức</v>
       </c>
-      <c r="O2" t="str">
+      <c r="P2" t="str">
         <v>1234567890</v>
       </c>
-      <c r="P2" t="str">
+      <c r="Q2" t="str">
         <v>VCB</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:P2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Q2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Add specialization/certificates to education, move bank info to contract section
</commit_message>
<xml_diff>
--- a/public/templates/employeeImportTemplate.xlsx
+++ b/public/templates/employeeImportTemplate.xlsx
@@ -397,14 +397,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Mã nhân viên *</v>
+        <v>Mã NV *</v>
       </c>
       <c r="B1" t="str">
         <v>Họ và tên *</v>
@@ -443,15 +443,21 @@
         <v>Trình độ học vấn</v>
       </c>
       <c r="N1" t="str">
+        <v>Chuyên ngành</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Chứng chỉ</v>
+      </c>
+      <c r="P1" t="str">
         <v>Ngày vào làm</v>
       </c>
-      <c r="O1" t="str">
+      <c r="Q1" t="str">
         <v>Loại hợp đồng</v>
       </c>
-      <c r="P1" t="str">
+      <c r="R1" t="str">
         <v>Số tài khoản NH</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="S1" t="str">
         <v>Tên ngân hàng</v>
       </c>
     </row>
@@ -496,21 +502,27 @@
         <v>Đại học</v>
       </c>
       <c r="N2" t="str">
+        <v>CNTT</v>
+      </c>
+      <c r="O2" t="str">
+        <v>PMP</v>
+      </c>
+      <c r="P2" t="str">
         <v>01/01/2024</v>
       </c>
-      <c r="O2" t="str">
-        <v>Chính thức</v>
-      </c>
-      <c r="P2" t="str">
+      <c r="Q2" t="str">
+        <v>Full-time</v>
+      </c>
+      <c r="R2" t="str">
         <v>1234567890</v>
       </c>
-      <c r="Q2" t="str">
+      <c r="S2" t="str">
         <v>VCB</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Q2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:S2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>